<commit_message>
added assets, documentation work
</commit_message>
<xml_diff>
--- a/Smart Light Gen2.xlsx
+++ b/Smart Light Gen2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="80" windowWidth="19140" windowHeight="6930" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="80" windowWidth="12850" windowHeight="5460" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Resource" sheetId="1" r:id="rId1"/>
@@ -14,13 +14,15 @@
     <sheet name="Packet Structure" sheetId="6" r:id="rId5"/>
     <sheet name="Command" sheetId="7" r:id="rId6"/>
     <sheet name="Payload" sheetId="5" r:id="rId7"/>
+    <sheet name="FOTA" sheetId="8" r:id="rId8"/>
+    <sheet name="JSON" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="319">
   <si>
     <t>S/N</t>
   </si>
@@ -669,6 +671,315 @@
   </si>
   <si>
     <t>Key16</t>
+  </si>
+  <si>
+    <t>Source ID is used for the packets from nodes</t>
+  </si>
+  <si>
+    <t>Destination ID is used for the packets from gateway/server</t>
+  </si>
+  <si>
+    <t>0x0026</t>
+  </si>
+  <si>
+    <t>0x0027</t>
+  </si>
+  <si>
+    <t>0x0028</t>
+  </si>
+  <si>
+    <t>0x0029</t>
+  </si>
+  <si>
+    <t>0x0030</t>
+  </si>
+  <si>
+    <t>0x002a</t>
+  </si>
+  <si>
+    <t>0x002b</t>
+  </si>
+  <si>
+    <t>0x002c</t>
+  </si>
+  <si>
+    <t>0x002d</t>
+  </si>
+  <si>
+    <t>0x002e</t>
+  </si>
+  <si>
+    <t>0x002f</t>
+  </si>
+  <si>
+    <t>0x0031</t>
+  </si>
+  <si>
+    <t>0x0032</t>
+  </si>
+  <si>
+    <t>0x0033</t>
+  </si>
+  <si>
+    <t>0x0034</t>
+  </si>
+  <si>
+    <t>0x0035</t>
+  </si>
+  <si>
+    <t>0x0036</t>
+  </si>
+  <si>
+    <t>0x0037</t>
+  </si>
+  <si>
+    <t>0x0038</t>
+  </si>
+  <si>
+    <t>0x0039</t>
+  </si>
+  <si>
+    <t>Motion Detected</t>
+  </si>
+  <si>
+    <t>0x003a</t>
+  </si>
+  <si>
+    <t>0x003b</t>
+  </si>
+  <si>
+    <t>0x003c</t>
+  </si>
+  <si>
+    <t>0x003d</t>
+  </si>
+  <si>
+    <t>0x003e</t>
+  </si>
+  <si>
+    <t>0x003f</t>
+  </si>
+  <si>
+    <t>Firmware update date set request</t>
+  </si>
+  <si>
+    <t>Firmware update date set response</t>
+  </si>
+  <si>
+    <t>Motion Trigger table</t>
+  </si>
+  <si>
+    <t>Contains all the allowed Zones</t>
+  </si>
+  <si>
+    <t>Contains all the allowed Groups</t>
+  </si>
+  <si>
+    <t>Contains all the allowed Source addresses</t>
+  </si>
+  <si>
+    <t>Contains all the allowed Destination addresses</t>
+  </si>
+  <si>
+    <t>Contains all the allowed motion triggers</t>
+  </si>
+  <si>
+    <t>0x15</t>
+  </si>
+  <si>
+    <t>example provision</t>
+  </si>
+  <si>
+    <t>0x00000000</t>
+  </si>
+  <si>
+    <t>0xabcd</t>
+  </si>
+  <si>
+    <t>0x00000001</t>
+  </si>
+  <si>
+    <t>0x00000011</t>
+  </si>
+  <si>
+    <t>0x0001</t>
+  </si>
+  <si>
+    <t>Get f/w version</t>
+  </si>
+  <si>
+    <t>Send image 1st packet</t>
+  </si>
+  <si>
+    <t>Steps for server</t>
+  </si>
+  <si>
+    <t>Steps for device</t>
+  </si>
+  <si>
+    <t>Send the existing f/w version</t>
+  </si>
+  <si>
+    <t>On receiving any packet, clear the new image magic number if it's not cleared and save the packet in flash/memory</t>
+  </si>
+  <si>
+    <t>Send image 2nd packet</t>
+  </si>
+  <si>
+    <t>..</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>Send image nth packet</t>
+  </si>
+  <si>
+    <t>Repeat image sending for 3 times</t>
+  </si>
+  <si>
+    <t>Request for missing images for individual devices</t>
+  </si>
+  <si>
+    <t>Send number of missing images</t>
+  </si>
+  <si>
+    <t>if missing image is more than 30%, repeat from 2 for 3 times</t>
+  </si>
+  <si>
+    <t>Request for number of missing packets</t>
+  </si>
+  <si>
+    <t>There will be 3 comlete retries and after that start communicating individually</t>
+  </si>
+  <si>
+    <t>Send first missing image</t>
+  </si>
+  <si>
+    <t>broadcast the missing image</t>
+  </si>
+  <si>
+    <t>repeat the query and broadcast untill all the images are saved successfully</t>
+  </si>
+  <si>
+    <t>If there are no missing image for the device, set the firmware upgrade date  and time</t>
+  </si>
+  <si>
+    <t>Save the firmware upgrade date and time</t>
+  </si>
+  <si>
+    <t>Save firmware upgrade date time set flag</t>
+  </si>
+  <si>
+    <t>Every hour if firmware upgrade date time flag is set, check the firmware upgrade date and time, if it matches, save firmware upgrade flag for boot loader and reboot. This will initiate the firmware upgrade process.</t>
+  </si>
+  <si>
+    <t>For individual device, get first 16 missing images</t>
+  </si>
+  <si>
+    <t>Get firmware version request</t>
+  </si>
+  <si>
+    <t>Get firmware version response</t>
+  </si>
+  <si>
+    <t>laterst firmware in server request</t>
+  </si>
+  <si>
+    <t>latest firmware in server response</t>
+  </si>
+  <si>
+    <t>0x0040</t>
+  </si>
+  <si>
+    <t>0x0041</t>
+  </si>
+  <si>
+    <t>0x0042</t>
+  </si>
+  <si>
+    <t>0x0043</t>
+  </si>
+  <si>
+    <t>0x0044</t>
+  </si>
+  <si>
+    <t>0x0045</t>
+  </si>
+  <si>
+    <t>0x0046</t>
+  </si>
+  <si>
+    <t>0x0047</t>
+  </si>
+  <si>
+    <t>0x0048</t>
+  </si>
+  <si>
+    <t>0x0049</t>
+  </si>
+  <si>
+    <t>Sensor data</t>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SenderId:"LightingSystem-AZTECH-11-GATEWAY", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SensorID:"LightingSystem-AZTECH-11-LoRa", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EventId:"EV-01-aa-bb", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EventType:"LightingSystem/variable#reading", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parameters:{ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">version:1, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">misc:0, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">counter:1, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">zone:1, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">group:1, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">misc1:0, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">destinationID:1, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sourceID:1, </t>
+  </si>
+  <si>
+    <t>command:32 ,</t>
+  </si>
+  <si>
+    <t>datasize:4 ,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">} </t>
+  </si>
+  <si>
+    <t>}"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time:"tttttttt", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">payload:"nnnn" </t>
   </si>
 </sst>
 </file>
@@ -712,7 +1023,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -725,6 +1036,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4998,10 +5310,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5009,11 +5321,11 @@
     <col min="2" max="2" width="22.36328125" customWidth="1"/>
     <col min="3" max="3" width="10.81640625" customWidth="1"/>
     <col min="4" max="4" width="10.6328125" customWidth="1"/>
-    <col min="9" max="9" width="13.26953125" customWidth="1"/>
+    <col min="9" max="9" width="17.81640625" customWidth="1"/>
     <col min="10" max="10" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5029,8 +5341,11 @@
       <c r="G1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="O1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5049,8 +5364,11 @@
       <c r="G2" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="O2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5069,8 +5387,11 @@
       <c r="G3" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="O3" s="6" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5081,7 +5402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5091,8 +5412,11 @@
       <c r="C5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="O5" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5105,8 +5429,11 @@
       <c r="G6" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="O6" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5116,8 +5443,11 @@
       <c r="C7">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="O7" s="6" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -5127,8 +5457,11 @@
       <c r="C8">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="O8" s="6" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -5138,13 +5471,19 @@
       <c r="C9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="O9" s="6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>93</v>
       </c>
@@ -5152,7 +5491,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
       <c r="I18" t="s">
         <v>120</v>
       </c>
@@ -5160,15 +5499,18 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
       <c r="I19" t="s">
         <v>121</v>
       </c>
       <c r="J19" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="L19" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>100</v>
       </c>
@@ -5181,8 +5523,11 @@
       <c r="J20" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="L20" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>102</v>
       </c>
@@ -5195,8 +5540,11 @@
       <c r="J21" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="L21" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>104</v>
       </c>
@@ -5209,8 +5557,22 @@
       <c r="J22" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="L22" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="I23" t="s">
+        <v>247</v>
+      </c>
+      <c r="J23" t="s">
+        <v>125</v>
+      </c>
+      <c r="L23" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>106</v>
       </c>
@@ -5218,7 +5580,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>108</v>
       </c>
@@ -5226,7 +5588,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>109</v>
       </c>
@@ -5234,7 +5596,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>111</v>
       </c>
@@ -5242,7 +5604,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>113</v>
       </c>
@@ -5250,7 +5612,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>115</v>
       </c>
@@ -5258,7 +5620,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>128</v>
       </c>
@@ -5268,28 +5630,34 @@
       <c r="E33" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="J33" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.35">
       <c r="E34" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.35">
       <c r="E35" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.35">
       <c r="E36" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
         <v>129</v>
       </c>
       <c r="C39" t="s">
         <v>130</v>
+      </c>
+      <c r="J39" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -5299,11 +5667,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5425,9 +5793,6 @@
       <c r="B10" t="s">
         <v>160</v>
       </c>
-      <c r="C10" t="s">
-        <v>177</v>
-      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
@@ -5436,9 +5801,6 @@
       <c r="B11" t="s">
         <v>161</v>
       </c>
-      <c r="C11" t="s">
-        <v>178</v>
-      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
@@ -5447,9 +5809,6 @@
       <c r="B12" t="s">
         <v>162</v>
       </c>
-      <c r="C12" t="s">
-        <v>179</v>
-      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
@@ -5458,9 +5817,6 @@
       <c r="B13" t="s">
         <v>163</v>
       </c>
-      <c r="C13" t="s">
-        <v>180</v>
-      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
@@ -5469,9 +5825,6 @@
       <c r="B14" t="s">
         <v>164</v>
       </c>
-      <c r="C14" t="s">
-        <v>181</v>
-      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
@@ -5480,9 +5833,6 @@
       <c r="B15" t="s">
         <v>165</v>
       </c>
-      <c r="C15" t="s">
-        <v>182</v>
-      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16">
@@ -5492,7 +5842,7 @@
         <v>148</v>
       </c>
       <c r="C16" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -5503,7 +5853,7 @@
         <v>149</v>
       </c>
       <c r="C17" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -5514,7 +5864,7 @@
         <v>150</v>
       </c>
       <c r="C18" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -5525,7 +5875,7 @@
         <v>151</v>
       </c>
       <c r="C19" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -5535,6 +5885,9 @@
       <c r="B20" t="s">
         <v>152</v>
       </c>
+      <c r="C20" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
@@ -5543,6 +5896,9 @@
       <c r="B21" t="s">
         <v>153</v>
       </c>
+      <c r="C21" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
@@ -5551,6 +5907,9 @@
       <c r="B22" t="s">
         <v>154</v>
       </c>
+      <c r="C22" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
@@ -5559,6 +5918,9 @@
       <c r="B23" t="s">
         <v>155</v>
       </c>
+      <c r="C23" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
@@ -5567,6 +5929,9 @@
       <c r="B24" t="s">
         <v>156</v>
       </c>
+      <c r="C24" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
@@ -5575,6 +5940,9 @@
       <c r="B25" t="s">
         <v>157</v>
       </c>
+      <c r="C25" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
@@ -5632,7 +6000,7 @@
         <v>158</v>
       </c>
       <c r="C32" t="s">
-        <v>191</v>
+        <v>284</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -5642,6 +6010,9 @@
       <c r="B33" t="s">
         <v>159</v>
       </c>
+      <c r="C33" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34">
@@ -5650,6 +6021,9 @@
       <c r="B34" t="s">
         <v>192</v>
       </c>
+      <c r="C34" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35">
@@ -5659,7 +6033,7 @@
         <v>193</v>
       </c>
       <c r="C35" t="s">
-        <v>196</v>
+        <v>287</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
@@ -5670,7 +6044,7 @@
         <v>194</v>
       </c>
       <c r="C36" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
@@ -5685,20 +6059,306 @@
       <c r="A38">
         <v>37</v>
       </c>
+      <c r="B38" t="s">
+        <v>218</v>
+      </c>
+      <c r="C38" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
+      <c r="B39" t="s">
+        <v>219</v>
+      </c>
+      <c r="C39" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
+      <c r="B40" t="s">
+        <v>220</v>
+      </c>
+      <c r="C40" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>221</v>
+      </c>
+      <c r="C41" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>288</v>
+      </c>
+      <c r="C64" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>290</v>
+      </c>
+      <c r="C66" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -5711,7 +6371,7 @@
   <dimension ref="A1:BU7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V7" sqref="V7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5729,10 +6389,10 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="6"/>
+      <c r="C1" s="7"/>
       <c r="D1" s="3">
         <v>1</v>
       </c>
@@ -5901,4 +6561,289 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="57.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="54.90625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B7" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B11" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B12" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B14" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B15" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="B17" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B20" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="B21" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C24" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="C25" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>316</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>